<commit_message>
Mess with Shadow map
</commit_message>
<xml_diff>
--- a/DX_study/DX_study/Data/CSV/Scene_GameObject.xlsx
+++ b/DX_study/DX_study/Data/CSV/Scene_GameObject.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\source\repos\2020_DirectX_Project\DX_study\DX_study\Data\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5988191-18D3-4858-A2A7-6B3DAB46A9F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C06F237-FB34-4DC3-BAE5-5C92627E57AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F553E549-D7D4-4838-9823-4E194DD1707F}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>skinned_vertex</t>
   </si>
   <si>
-    <t>Box</t>
-  </si>
-  <si>
     <t>Ground</t>
   </si>
   <si>
@@ -105,6 +102,10 @@
   </si>
   <si>
     <t>CharacterMove/Animator</t>
+  </si>
+  <si>
+    <t>Sphere</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -557,7 +558,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -573,118 +574,118 @@
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>